<commit_message>
Popravila scenarij i tok dogadjaja za registriranje korisnika, u dijelu glavnih aktera (Korisnik->Glavni korisnik)
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/Registriranje na sistem.xlsx
+++ b/UseCaseIScenarij/Registriranje na sistem.xlsx
@@ -45,9 +45,6 @@
     <t>Glavni tok</t>
   </si>
   <si>
-    <t>Korisnik alarm sistema</t>
-  </si>
-  <si>
     <t>Tok događaja:</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t xml:space="preserve">Korisnik nije uspjesno registriran na sistem zabog nevalidnih podataka ili neke druge greske </t>
   </si>
   <si>
-    <t>Korisnik alarm sistema i sistem za registraciju korisnika</t>
-  </si>
-  <si>
     <t>/</t>
   </si>
   <si>
@@ -127,6 +121,12 @@
   </si>
   <si>
     <t>4. Ponuda za novo unosenje podataka</t>
+  </si>
+  <si>
+    <t>Glavni korisnik alarm sistema</t>
+  </si>
+  <si>
+    <t>Glavni korisnik alarm sistema i sistem za registraciju korisnika</t>
   </si>
 </sst>
 </file>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -530,7 +530,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="46.5" customHeight="1">
@@ -538,7 +538,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="82.5" customHeight="1">
@@ -546,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="75.75" customHeight="1">
@@ -554,7 +554,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="49.5" customHeight="1">
@@ -562,7 +562,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="41.25" customHeight="1">
@@ -570,7 +570,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="54" customHeight="1">
@@ -578,15 +578,15 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="33.75" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="36.75" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="60" customHeight="1">
@@ -594,7 +594,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="61.5" customHeight="1">
@@ -602,40 +602,40 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="36" customHeight="1">
       <c r="A17" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3" ht="21.75" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="7"/>
     </row>
@@ -643,74 +643,74 @@
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="1" customFormat="1" ht="69" customHeight="1">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="1" customFormat="1" ht="69" customHeight="1">
       <c r="A21" s="11"/>
       <c r="B21" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" s="11"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="30.75" customHeight="1">
       <c r="A27" s="10" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B27" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="7"/>
       <c r="B28" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" ht="51.75" customHeight="1">
       <c r="A29" s="7"/>
       <c r="B29" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:3" ht="31.5" customHeight="1">
       <c r="A30" s="7"/>
       <c r="B30" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:3" ht="33.75" customHeight="1">
       <c r="A31" s="7"/>
       <c r="B31" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C31" s="7"/>
     </row>

</xml_diff>